<commit_message>
Modified encoder dash and modifed some query in stdudent subs
</commit_message>
<xml_diff>
--- a/Resources/PL101.xlsx
+++ b/Resources/PL101.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>NAME</t>
   </si>
@@ -126,13 +126,61 @@
   </si>
   <si>
     <t>3rd year</t>
+  </si>
+  <si>
+    <t>ACEBEEDO, ABCDE CZARRINA ERIKA</t>
+  </si>
+  <si>
+    <t>ALARO, MARIA CRISTINA</t>
+  </si>
+  <si>
+    <t>BADAL, ROSELYN</t>
+  </si>
+  <si>
+    <t>BALOSA, JOHN RAY V</t>
+  </si>
+  <si>
+    <t>CABALDA, RECCA ANN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABRERA, ROMMEL </t>
+  </si>
+  <si>
+    <t>DALIT, JOHN CARLO F</t>
+  </si>
+  <si>
+    <t>DISTOR, LENZER ELEE T</t>
+  </si>
+  <si>
+    <t>Duran, Kenneth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GARCIA, KHRISTINE ANNE LOUISE  </t>
+  </si>
+  <si>
+    <t>MONDARES, JASONN D</t>
+  </si>
+  <si>
+    <t>RABINA, PAUL JUSTINE</t>
+  </si>
+  <si>
+    <t>SABALZA, VINA D</t>
+  </si>
+  <si>
+    <t>SAMANIEGO, MATTHEW V</t>
+  </si>
+  <si>
+    <t>SATUR, JOHN MARC</t>
+  </si>
+  <si>
+    <t>4th year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +202,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -163,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -171,11 +231,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -186,6 +274,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F32"/>
+  <dimension ref="A3:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +911,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -816,11 +922,178 @@
         <v>88</v>
       </c>
     </row>
+    <row r="33" spans="1:3" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="9">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:F3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>